<commit_message>
primary function of diagnosis
</commit_message>
<xml_diff>
--- a/src/app/projects/hyponatremia/ram_db/db.xlsx
+++ b/src/app/projects/hyponatremia/ram_db/db.xlsx
@@ -528,7 +528,7 @@
         <v>男/女</v>
       </c>
       <c r="C3" t="str">
-        <v>Family History</v>
+        <v>Family</v>
       </c>
       <c r="D3" t="str">
         <v>家族病史</v>
@@ -587,7 +587,7 @@
         <v>病人主訴</v>
       </c>
       <c r="C4" t="str">
-        <v>Travel History</v>
+        <v>Travel</v>
       </c>
       <c r="D4" t="str">
         <v>旅遊史</v>

</xml_diff>

<commit_message>
fixed some unit problems
</commit_message>
<xml_diff>
--- a/src/app/projects/hyponatremia/ram_db/db.xlsx
+++ b/src/app/projects/hyponatremia/ram_db/db.xlsx
@@ -521,31 +521,31 @@
         <v>ChestI</v>
       </c>
       <c r="J2" t="str">
-        <v>Chest I</v>
+        <v>胸部視診</v>
       </c>
       <c r="K2" t="str">
         <v>ChestA</v>
       </c>
       <c r="L2" t="str">
-        <v>Chest A</v>
+        <v>胸部聽診</v>
       </c>
       <c r="M2" t="str">
         <v>ChestPe</v>
       </c>
       <c r="N2" t="str">
-        <v>Chest Pe</v>
+        <v>胸部扣診</v>
       </c>
       <c r="O2" t="str">
         <v>ChestPa</v>
       </c>
       <c r="P2" t="str">
-        <v>Chest Pa</v>
+        <v>胸部觸診</v>
       </c>
       <c r="Q2" t="str">
         <v>ChestCT</v>
       </c>
       <c r="R2" t="str">
-        <v>Chest Xray and CT</v>
+        <v>胸部X光與電腦斷層</v>
       </c>
       <c r="S2" t="str">
         <v>RBC</v>
@@ -610,25 +610,25 @@
         <v>AbdomenI</v>
       </c>
       <c r="J3" t="str">
-        <v>Abdomen I</v>
+        <v>腹部視診</v>
       </c>
       <c r="K3" t="str">
         <v>AbdomenA</v>
       </c>
       <c r="L3" t="str">
-        <v>Abdomen A</v>
+        <v>腹部聽診</v>
       </c>
       <c r="M3" t="str">
         <v>AbdomenPe</v>
       </c>
       <c r="N3" t="str">
-        <v>Abdomen Pe</v>
+        <v>腹部扣診</v>
       </c>
       <c r="O3" t="str">
         <v>AbdomenPa</v>
       </c>
       <c r="P3" t="str">
-        <v>Abdomen Pa</v>
+        <v>腹部觸診</v>
       </c>
       <c r="Q3" t="str">
         <v>AbdSono</v>
@@ -652,7 +652,7 @@
         <v>PCO2</v>
       </c>
       <c r="X3" t="str">
-        <v>CO2 Partial Pressure</v>
+        <v>二氧化碳分壓 (PCO2)</v>
       </c>
       <c r="Y3" t="str">
         <v>Q2</v>
@@ -699,7 +699,25 @@
         <v>ExtremetiesI</v>
       </c>
       <c r="J4" t="str">
-        <v>Extremeties I</v>
+        <v>四肢視診</v>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+      <c r="O4" t="str">
+        <v/>
+      </c>
+      <c r="P4" t="str">
+        <v/>
       </c>
       <c r="Q4" t="str">
         <v>ThySono</v>
@@ -723,7 +741,7 @@
         <v>PO2</v>
       </c>
       <c r="X4" t="str">
-        <v>Oxygen Partial Pressure</v>
+        <v>氧分壓 (PO2)</v>
       </c>
       <c r="Y4" t="str">
         <v>Q3</v>
@@ -770,19 +788,37 @@
         <v>HEENTI</v>
       </c>
       <c r="J5" t="str">
-        <v>HEENT I</v>
+        <v>頭頸視診</v>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <v/>
       </c>
       <c r="Q5" t="str">
         <v>HeadCT</v>
       </c>
       <c r="R5" t="str">
-        <v>CT Scan of head</v>
+        <v>頭部電腦斷層</v>
       </c>
       <c r="S5" t="str">
         <v>Na</v>
       </c>
       <c r="T5" t="str">
-        <v>Na</v>
+        <v>血鈉</v>
       </c>
       <c r="U5" t="str">
         <v>Glucose</v>
@@ -794,7 +830,7 @@
         <v>SO2</v>
       </c>
       <c r="X5" t="str">
-        <v>Oxygen Saturation</v>
+        <v>血氧飽和度 (SO2)</v>
       </c>
       <c r="Y5" t="str">
         <v>Q4</v>
@@ -841,13 +877,37 @@
         <v>GenitourinaryI</v>
       </c>
       <c r="J6" t="str">
-        <v>Genitourinary I</v>
+        <v>泌尿生殖視診</v>
+      </c>
+      <c r="K6" t="str">
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <v/>
+      </c>
+      <c r="O6" t="str">
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <v/>
+      </c>
+      <c r="Q6" t="str">
+        <v/>
+      </c>
+      <c r="R6" t="str">
+        <v/>
       </c>
       <c r="S6" t="str">
         <v>K</v>
       </c>
       <c r="T6" t="str">
-        <v>K</v>
+        <v>血鉀</v>
       </c>
       <c r="U6" t="str">
         <v>Protein</v>
@@ -859,7 +919,7 @@
         <v>HCO3</v>
       </c>
       <c r="X6" t="str">
-        <v>Bicarbonate</v>
+        <v>血液重碳酸鹽 (HCO3)</v>
       </c>
       <c r="Y6" t="str">
         <v>Q5</v>
@@ -888,19 +948,55 @@
         <v>Location</v>
       </c>
       <c r="D7" t="str">
-        <v>Location</v>
+        <v>位置</v>
       </c>
       <c r="E7" t="str">
         <v/>
       </c>
       <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <v/>
+      </c>
+      <c r="Q7" t="str">
+        <v/>
+      </c>
+      <c r="R7" t="str">
         <v/>
       </c>
       <c r="S7" t="str">
         <v>Cl</v>
       </c>
       <c r="T7" t="str">
-        <v>Cl</v>
+        <v>血氯</v>
       </c>
       <c r="U7" t="str">
         <v>OB</v>
@@ -912,7 +1008,7 @@
         <v>BE</v>
       </c>
       <c r="X7" t="str">
-        <v>Base Excess</v>
+        <v>鹼超量 (Base excess)</v>
       </c>
       <c r="Y7" t="str">
         <v>Q6</v>
@@ -941,25 +1037,67 @@
         <v>Quality</v>
       </c>
       <c r="D8" t="str">
-        <v>Quality</v>
+        <v>型態</v>
       </c>
       <c r="E8" t="str">
         <v/>
       </c>
       <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <v/>
+      </c>
+      <c r="Q8" t="str">
+        <v/>
+      </c>
+      <c r="R8" t="str">
         <v/>
       </c>
       <c r="S8" t="str">
         <v>Mg</v>
       </c>
       <c r="T8" t="str">
-        <v>Mg</v>
+        <v>血鎂</v>
       </c>
       <c r="U8" t="str">
         <v>RBC</v>
       </c>
       <c r="V8" t="str">
         <v>紅血球</v>
+      </c>
+      <c r="W8" t="str">
+        <v/>
+      </c>
+      <c r="X8" t="str">
+        <v/>
       </c>
       <c r="Y8" t="str">
         <v>Q7</v>
@@ -988,25 +1126,67 @@
         <v>Quantity</v>
       </c>
       <c r="D9" t="str">
-        <v>Quantity</v>
+        <v>歷時長短</v>
       </c>
       <c r="E9" t="str">
         <v/>
       </c>
       <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v/>
+      </c>
+      <c r="O9" t="str">
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <v/>
+      </c>
+      <c r="Q9" t="str">
+        <v/>
+      </c>
+      <c r="R9" t="str">
         <v/>
       </c>
       <c r="S9" t="str">
         <v>Ca</v>
       </c>
       <c r="T9" t="str">
-        <v>Ca</v>
+        <v>血鈣</v>
       </c>
       <c r="U9" t="str">
         <v>WBC</v>
       </c>
       <c r="V9" t="str">
         <v>白血球</v>
+      </c>
+      <c r="W9" t="str">
+        <v/>
+      </c>
+      <c r="X9" t="str">
+        <v/>
       </c>
       <c r="Y9" t="str">
         <v>Q8</v>
@@ -1035,7 +1215,7 @@
         <v>Onset mode</v>
       </c>
       <c r="D10" t="str">
-        <v>Onset mode</v>
+        <v>發作形式</v>
       </c>
       <c r="E10" t="str">
         <v/>
@@ -1043,17 +1223,59 @@
       <c r="F10" t="str">
         <v/>
       </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v/>
+      </c>
+      <c r="O10" t="str">
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <v/>
+      </c>
+      <c r="Q10" t="str">
+        <v/>
+      </c>
+      <c r="R10" t="str">
+        <v/>
+      </c>
       <c r="S10" t="str">
-        <v>Osmolality</v>
+        <v>Osmolarity</v>
       </c>
       <c r="T10" t="str">
-        <v>Plasma Osmolality</v>
+        <v>血漿滲透壓</v>
       </c>
       <c r="U10" t="str">
         <v>Na</v>
       </c>
       <c r="V10" t="str">
-        <v>Na</v>
+        <v>尿鈉</v>
+      </c>
+      <c r="W10" t="str">
+        <v/>
+      </c>
+      <c r="X10" t="str">
+        <v/>
       </c>
       <c r="Y10" t="str">
         <v>Q9</v>
@@ -1082,25 +1304,67 @@
         <v>PrecipitatingFactors</v>
       </c>
       <c r="D11" t="str">
-        <v>Precipitating Factors</v>
+        <v>情境或誘發因素</v>
       </c>
       <c r="E11" t="str">
         <v/>
       </c>
       <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v/>
+      </c>
+      <c r="O11" t="str">
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <v/>
+      </c>
+      <c r="Q11" t="str">
+        <v/>
+      </c>
+      <c r="R11" t="str">
         <v/>
       </c>
       <c r="S11" t="str">
         <v>BUN</v>
       </c>
       <c r="T11" t="str">
-        <v>BUN</v>
+        <v>血液尿素氮 (BUN)</v>
       </c>
       <c r="U11" t="str">
         <v>K</v>
       </c>
       <c r="V11" t="str">
-        <v>K</v>
+        <v>尿鉀</v>
+      </c>
+      <c r="W11" t="str">
+        <v/>
+      </c>
+      <c r="X11" t="str">
+        <v/>
       </c>
       <c r="Y11" t="str">
         <v>Q10</v>
@@ -1129,25 +1393,67 @@
         <v>ExaggeratingFactors</v>
       </c>
       <c r="D12" t="str">
-        <v>Exaggerating Factors</v>
+        <v>加重因素</v>
       </c>
       <c r="E12" t="str">
         <v/>
       </c>
       <c r="F12" t="str">
+        <v/>
+      </c>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v/>
+      </c>
+      <c r="O12" t="str">
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <v/>
+      </c>
+      <c r="Q12" t="str">
+        <v/>
+      </c>
+      <c r="R12" t="str">
         <v/>
       </c>
       <c r="S12" t="str">
         <v>Creatinine</v>
       </c>
       <c r="T12" t="str">
-        <v>Creatinine</v>
+        <v>血液肌酸酐 (Creatinine)</v>
       </c>
       <c r="U12" t="str">
         <v>Creatinine</v>
       </c>
       <c r="V12" t="str">
-        <v>Creatinine</v>
+        <v>尿液肌酸酐 (Creatinine)</v>
+      </c>
+      <c r="W12" t="str">
+        <v/>
+      </c>
+      <c r="X12" t="str">
+        <v/>
       </c>
       <c r="Y12" t="str">
         <v>Q11</v>
@@ -1176,12 +1482,48 @@
         <v>RelievingFactors</v>
       </c>
       <c r="D13" t="str">
-        <v>Relieving Factors</v>
+        <v>緩解因素</v>
       </c>
       <c r="E13" t="str">
         <v/>
       </c>
       <c r="F13" t="str">
+        <v/>
+      </c>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <v/>
+      </c>
+      <c r="Q13" t="str">
+        <v/>
+      </c>
+      <c r="R13" t="str">
         <v/>
       </c>
       <c r="S13" t="str">
@@ -1191,10 +1533,16 @@
         <v>eGFR</v>
       </c>
       <c r="U13" t="str">
-        <v>Osmolality</v>
+        <v>Osmolarity</v>
       </c>
       <c r="V13" t="str">
-        <v>Urine Osmolality</v>
+        <v>尿液滲透壓</v>
+      </c>
+      <c r="W13" t="str">
+        <v/>
+      </c>
+      <c r="X13" t="str">
+        <v/>
       </c>
       <c r="Y13" t="str">
         <v>Q12</v>
@@ -1223,12 +1571,48 @@
         <v>AccompanyingSymptoms</v>
       </c>
       <c r="D14" t="str">
-        <v>Accompanying Symptoms</v>
+        <v>伴隨症狀</v>
       </c>
       <c r="E14" t="str">
         <v/>
       </c>
       <c r="F14" t="str">
+        <v/>
+      </c>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <v/>
+      </c>
+      <c r="P14" t="str">
+        <v/>
+      </c>
+      <c r="Q14" t="str">
+        <v/>
+      </c>
+      <c r="R14" t="str">
         <v/>
       </c>
       <c r="S14" t="str">
@@ -1241,7 +1625,13 @@
         <v>Gravity</v>
       </c>
       <c r="V14" t="str">
-        <v>Urine Specific Gravity</v>
+        <v>尿液比重</v>
+      </c>
+      <c r="W14" t="str">
+        <v/>
+      </c>
+      <c r="X14" t="str">
+        <v/>
       </c>
       <c r="Y14" t="str">
         <v>Q13</v>
@@ -1266,10 +1656,52 @@
       <c r="B15" t="str">
         <v>60</v>
       </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
       <c r="E15" t="str">
         <v/>
       </c>
       <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <v/>
+      </c>
+      <c r="O15" t="str">
+        <v/>
+      </c>
+      <c r="P15" t="str">
+        <v/>
+      </c>
+      <c r="Q15" t="str">
+        <v/>
+      </c>
+      <c r="R15" t="str">
         <v/>
       </c>
       <c r="S15" t="str">
@@ -1278,6 +1710,18 @@
       <c r="T15" t="str">
         <v>T3</v>
       </c>
+      <c r="U15" t="str">
+        <v>Clarity</v>
+      </c>
+      <c r="V15" t="str">
+        <v>Clarity/tubidity</v>
+      </c>
+      <c r="W15" t="str">
+        <v/>
+      </c>
+      <c r="X15" t="str">
+        <v/>
+      </c>
       <c r="Y15" t="str">
         <v>Q14</v>
       </c>
@@ -1295,10 +1739,58 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="str">
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
       <c r="E16" t="str">
         <v/>
       </c>
       <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16" t="str">
+        <v/>
+      </c>
+      <c r="O16" t="str">
+        <v/>
+      </c>
+      <c r="P16" t="str">
+        <v/>
+      </c>
+      <c r="Q16" t="str">
+        <v/>
+      </c>
+      <c r="R16" t="str">
         <v/>
       </c>
       <c r="S16" t="str">
@@ -1307,6 +1799,18 @@
       <c r="T16" t="str">
         <v>T4</v>
       </c>
+      <c r="U16" t="str">
+        <v/>
+      </c>
+      <c r="V16" t="str">
+        <v/>
+      </c>
+      <c r="W16" t="str">
+        <v/>
+      </c>
+      <c r="X16" t="str">
+        <v/>
+      </c>
       <c r="Y16" t="str">
         <v>Q15</v>
       </c>
@@ -1324,10 +1828,58 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
       <c r="E17" t="str">
         <v/>
       </c>
       <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17" t="str">
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <v/>
+      </c>
+      <c r="Q17" t="str">
+        <v/>
+      </c>
+      <c r="R17" t="str">
         <v/>
       </c>
       <c r="S17" t="str">
@@ -1336,6 +1888,18 @@
       <c r="T17" t="str">
         <v>ACTH</v>
       </c>
+      <c r="U17" t="str">
+        <v/>
+      </c>
+      <c r="V17" t="str">
+        <v/>
+      </c>
+      <c r="W17" t="str">
+        <v/>
+      </c>
+      <c r="X17" t="str">
+        <v/>
+      </c>
       <c r="Y17" t="str">
         <v>Q16</v>
       </c>
@@ -1353,10 +1917,58 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="str">
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
       <c r="E18" t="str">
         <v/>
       </c>
       <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
+      <c r="Q18" t="str">
+        <v/>
+      </c>
+      <c r="R18" t="str">
         <v/>
       </c>
       <c r="S18" t="str">
@@ -1365,6 +1977,18 @@
       <c r="T18" t="str">
         <v>GOT</v>
       </c>
+      <c r="U18" t="str">
+        <v/>
+      </c>
+      <c r="V18" t="str">
+        <v/>
+      </c>
+      <c r="W18" t="str">
+        <v/>
+      </c>
+      <c r="X18" t="str">
+        <v/>
+      </c>
       <c r="Y18" t="str">
         <v>Q17</v>
       </c>
@@ -1382,10 +2006,58 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="str">
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
       <c r="E19" t="str">
         <v/>
       </c>
       <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <v/>
+      </c>
+      <c r="J19" t="str">
+        <v/>
+      </c>
+      <c r="K19" t="str">
+        <v/>
+      </c>
+      <c r="L19" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <v/>
+      </c>
+      <c r="Q19" t="str">
+        <v/>
+      </c>
+      <c r="R19" t="str">
         <v/>
       </c>
       <c r="S19" t="str">
@@ -1394,6 +2066,18 @@
       <c r="T19" t="str">
         <v>GPT</v>
       </c>
+      <c r="U19" t="str">
+        <v/>
+      </c>
+      <c r="V19" t="str">
+        <v/>
+      </c>
+      <c r="W19" t="str">
+        <v/>
+      </c>
+      <c r="X19" t="str">
+        <v/>
+      </c>
       <c r="Y19" t="str">
         <v>Q18</v>
       </c>
@@ -1411,10 +2095,58 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="str">
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <v/>
+      </c>
+      <c r="C20" t="str">
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
       <c r="E20" t="str">
         <v/>
       </c>
       <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <v/>
+      </c>
+      <c r="I20" t="str">
+        <v/>
+      </c>
+      <c r="J20" t="str">
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <v/>
+      </c>
+      <c r="L20" t="str">
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <v/>
+      </c>
+      <c r="N20" t="str">
+        <v/>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <v/>
+      </c>
+      <c r="Q20" t="str">
+        <v/>
+      </c>
+      <c r="R20" t="str">
         <v/>
       </c>
       <c r="S20" t="str">
@@ -1423,6 +2155,18 @@
       <c r="T20" t="str">
         <v>血蛋白</v>
       </c>
+      <c r="U20" t="str">
+        <v/>
+      </c>
+      <c r="V20" t="str">
+        <v/>
+      </c>
+      <c r="W20" t="str">
+        <v/>
+      </c>
+      <c r="X20" t="str">
+        <v/>
+      </c>
       <c r="Y20" t="str">
         <v>Q19</v>
       </c>
@@ -1440,10 +2184,58 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="str">
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <v/>
+      </c>
+      <c r="C21" t="str">
+        <v/>
+      </c>
+      <c r="D21" t="str">
+        <v/>
+      </c>
       <c r="E21" t="str">
         <v/>
       </c>
       <c r="F21" t="str">
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <v/>
+      </c>
+      <c r="I21" t="str">
+        <v/>
+      </c>
+      <c r="J21" t="str">
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <v/>
+      </c>
+      <c r="L21" t="str">
+        <v/>
+      </c>
+      <c r="M21" t="str">
+        <v/>
+      </c>
+      <c r="N21" t="str">
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <v/>
+      </c>
+      <c r="Q21" t="str">
+        <v/>
+      </c>
+      <c r="R21" t="str">
         <v/>
       </c>
       <c r="S21" t="str">
@@ -1452,6 +2244,18 @@
       <c r="T21" t="str">
         <v>血糖</v>
       </c>
+      <c r="U21" t="str">
+        <v/>
+      </c>
+      <c r="V21" t="str">
+        <v/>
+      </c>
+      <c r="W21" t="str">
+        <v/>
+      </c>
+      <c r="X21" t="str">
+        <v/>
+      </c>
       <c r="Y21" t="str">
         <v>Q20</v>
       </c>
@@ -1469,10 +2273,58 @@
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="str">
+        <v/>
+      </c>
+      <c r="B22" t="str">
+        <v/>
+      </c>
+      <c r="C22" t="str">
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <v/>
+      </c>
       <c r="E22" t="str">
         <v/>
       </c>
       <c r="F22" t="str">
+        <v/>
+      </c>
+      <c r="G22" t="str">
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <v/>
+      </c>
+      <c r="I22" t="str">
+        <v/>
+      </c>
+      <c r="J22" t="str">
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <v/>
+      </c>
+      <c r="N22" t="str">
+        <v/>
+      </c>
+      <c r="O22" t="str">
+        <v/>
+      </c>
+      <c r="P22" t="str">
+        <v/>
+      </c>
+      <c r="Q22" t="str">
+        <v/>
+      </c>
+      <c r="R22" t="str">
         <v/>
       </c>
       <c r="S22" t="str">
@@ -1481,12 +2333,87 @@
       <c r="T22" t="str">
         <v>總膽紅素</v>
       </c>
+      <c r="U22" t="str">
+        <v/>
+      </c>
+      <c r="V22" t="str">
+        <v/>
+      </c>
+      <c r="W22" t="str">
+        <v/>
+      </c>
+      <c r="X22" t="str">
+        <v/>
+      </c>
+      <c r="Y22" t="str">
+        <v/>
+      </c>
+      <c r="Z22" t="str">
+        <v/>
+      </c>
+      <c r="AA22" t="str">
+        <v/>
+      </c>
+      <c r="AB22" t="str">
+        <v/>
+      </c>
+      <c r="AC22" t="str">
+        <v/>
+      </c>
     </row>
     <row r="23">
+      <c r="A23" t="str">
+        <v/>
+      </c>
+      <c r="B23" t="str">
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
       <c r="E23" t="str">
         <v/>
       </c>
       <c r="F23" t="str">
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <v/>
+      </c>
+      <c r="J23" t="str">
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <v/>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
+      <c r="Q23" t="str">
+        <v/>
+      </c>
+      <c r="R23" t="str">
         <v/>
       </c>
       <c r="S23" t="str">
@@ -1494,6 +2421,33 @@
       </c>
       <c r="T23" t="str">
         <v>糖化血色素</v>
+      </c>
+      <c r="U23" t="str">
+        <v/>
+      </c>
+      <c r="V23" t="str">
+        <v/>
+      </c>
+      <c r="W23" t="str">
+        <v/>
+      </c>
+      <c r="X23" t="str">
+        <v/>
+      </c>
+      <c r="Y23" t="str">
+        <v/>
+      </c>
+      <c r="Z23" t="str">
+        <v/>
+      </c>
+      <c r="AA23" t="str">
+        <v/>
+      </c>
+      <c r="AB23" t="str">
+        <v/>
+      </c>
+      <c r="AC23" t="str">
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -2226,6 +3180,24 @@
       <c r="N4" t="str">
         <v>No significant findings</v>
       </c>
+      <c r="O4" t="str">
+        <v/>
+      </c>
+      <c r="P4" t="str">
+        <v/>
+      </c>
+      <c r="Q4" t="str">
+        <v/>
+      </c>
+      <c r="R4" t="str">
+        <v/>
+      </c>
+      <c r="S4" t="str">
+        <v/>
+      </c>
+      <c r="T4" t="str">
+        <v/>
+      </c>
       <c r="U4" t="str">
         <v>ThySono</v>
       </c>
@@ -2239,7 +3211,7 @@
         <v>300</v>
       </c>
       <c r="Y4" t="str">
-        <v>Clarity/turbidity</v>
+        <v>Clarity</v>
       </c>
       <c r="Z4" t="str">
         <v>Clear</v>
@@ -2297,6 +3269,24 @@
       <c r="N5" t="str">
         <v>No significant findings</v>
       </c>
+      <c r="O5" t="str">
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <v/>
+      </c>
+      <c r="Q5" t="str">
+        <v/>
+      </c>
+      <c r="R5" t="str">
+        <v/>
+      </c>
+      <c r="S5" t="str">
+        <v/>
+      </c>
+      <c r="T5" t="str">
+        <v/>
+      </c>
       <c r="U5" t="str">
         <v>HeadCT</v>
       </c>
@@ -2368,6 +3358,30 @@
       <c r="N6" t="str">
         <v>No significant findings</v>
       </c>
+      <c r="O6" t="str">
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <v/>
+      </c>
+      <c r="Q6" t="str">
+        <v/>
+      </c>
+      <c r="R6" t="str">
+        <v/>
+      </c>
+      <c r="S6" t="str">
+        <v/>
+      </c>
+      <c r="T6" t="str">
+        <v/>
+      </c>
+      <c r="U6" t="str">
+        <v/>
+      </c>
+      <c r="V6" t="str">
+        <v/>
+      </c>
       <c r="W6" t="str">
         <v>K</v>
       </c>
@@ -2409,6 +3423,12 @@
       <c r="F7" t="str">
         <v/>
       </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
       <c r="I7" t="str">
         <v>Q6</v>
       </c>
@@ -2420,6 +3440,36 @@
       </c>
       <c r="L7" t="str">
         <v>沒有</v>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <v/>
+      </c>
+      <c r="Q7" t="str">
+        <v/>
+      </c>
+      <c r="R7" t="str">
+        <v/>
+      </c>
+      <c r="S7" t="str">
+        <v/>
+      </c>
+      <c r="T7" t="str">
+        <v/>
+      </c>
+      <c r="U7" t="str">
+        <v/>
+      </c>
+      <c r="V7" t="str">
+        <v/>
       </c>
       <c r="W7" t="str">
         <v>Cl</v>
@@ -2462,6 +3512,54 @@
       <c r="F8" t="str">
         <v/>
       </c>
+      <c r="G8" t="str">
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <v/>
+      </c>
+      <c r="Q8" t="str">
+        <v/>
+      </c>
+      <c r="R8" t="str">
+        <v/>
+      </c>
+      <c r="S8" t="str">
+        <v/>
+      </c>
+      <c r="T8" t="str">
+        <v/>
+      </c>
+      <c r="U8" t="str">
+        <v/>
+      </c>
+      <c r="V8" t="str">
+        <v/>
+      </c>
       <c r="W8" t="str">
         <v>Osmolarity</v>
       </c>
@@ -2473,6 +3571,12 @@
       </c>
       <c r="Z8" t="str">
         <v>Negative</v>
+      </c>
+      <c r="AA8" t="str">
+        <v/>
+      </c>
+      <c r="AB8" t="str">
+        <v/>
       </c>
       <c r="AC8" t="str">
         <v>GlucocorticoidDeficiency</v>
@@ -2497,6 +3601,54 @@
       <c r="F9" t="str">
         <v/>
       </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v/>
+      </c>
+      <c r="O9" t="str">
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <v/>
+      </c>
+      <c r="Q9" t="str">
+        <v/>
+      </c>
+      <c r="R9" t="str">
+        <v/>
+      </c>
+      <c r="S9" t="str">
+        <v/>
+      </c>
+      <c r="T9" t="str">
+        <v/>
+      </c>
+      <c r="U9" t="str">
+        <v/>
+      </c>
+      <c r="V9" t="str">
+        <v/>
+      </c>
       <c r="W9" t="str">
         <v>BUN</v>
       </c>
@@ -2508,6 +3660,12 @@
       </c>
       <c r="Z9" t="str">
         <v>Negative</v>
+      </c>
+      <c r="AA9" t="str">
+        <v/>
+      </c>
+      <c r="AB9" t="str">
+        <v/>
       </c>
       <c r="AC9" t="str">
         <v>PsychogenicPolydipsia</v>
@@ -2532,6 +3690,54 @@
       <c r="F10" t="str">
         <v/>
       </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v/>
+      </c>
+      <c r="O10" t="str">
+        <v/>
+      </c>
+      <c r="P10" t="str">
+        <v/>
+      </c>
+      <c r="Q10" t="str">
+        <v/>
+      </c>
+      <c r="R10" t="str">
+        <v/>
+      </c>
+      <c r="S10" t="str">
+        <v/>
+      </c>
+      <c r="T10" t="str">
+        <v/>
+      </c>
+      <c r="U10" t="str">
+        <v/>
+      </c>
+      <c r="V10" t="str">
+        <v/>
+      </c>
       <c r="W10" t="str">
         <v>Creatinine</v>
       </c>
@@ -2543,6 +3749,12 @@
       </c>
       <c r="Z10" t="str">
         <v>Negative</v>
+      </c>
+      <c r="AA10" t="str">
+        <v/>
+      </c>
+      <c r="AB10" t="str">
+        <v/>
       </c>
       <c r="AC10" t="str">
         <v>LowSolute</v>
@@ -2567,6 +3779,54 @@
       <c r="F11" t="str">
         <v/>
       </c>
+      <c r="G11" t="str">
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <v/>
+      </c>
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v/>
+      </c>
+      <c r="O11" t="str">
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <v/>
+      </c>
+      <c r="Q11" t="str">
+        <v/>
+      </c>
+      <c r="R11" t="str">
+        <v/>
+      </c>
+      <c r="S11" t="str">
+        <v/>
+      </c>
+      <c r="T11" t="str">
+        <v/>
+      </c>
+      <c r="U11" t="str">
+        <v/>
+      </c>
+      <c r="V11" t="str">
+        <v/>
+      </c>
       <c r="W11" t="str">
         <v>EGFR</v>
       </c>
@@ -2578,6 +3838,12 @@
       </c>
       <c r="Z11" t="str">
         <v>66</v>
+      </c>
+      <c r="AA11" t="str">
+        <v/>
+      </c>
+      <c r="AB11" t="str">
+        <v/>
       </c>
       <c r="AC11" t="str">
         <v>ChronicHeartFailure</v>
@@ -2602,6 +3868,54 @@
       <c r="F12" t="str">
         <v/>
       </c>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v/>
+      </c>
+      <c r="O12" t="str">
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <v/>
+      </c>
+      <c r="Q12" t="str">
+        <v/>
+      </c>
+      <c r="R12" t="str">
+        <v/>
+      </c>
+      <c r="S12" t="str">
+        <v/>
+      </c>
+      <c r="T12" t="str">
+        <v/>
+      </c>
+      <c r="U12" t="str">
+        <v/>
+      </c>
+      <c r="V12" t="str">
+        <v/>
+      </c>
       <c r="W12" t="str">
         <v>TSH</v>
       </c>
@@ -2613,6 +3927,12 @@
       </c>
       <c r="Z12" t="str">
         <v>17.5</v>
+      </c>
+      <c r="AA12" t="str">
+        <v/>
+      </c>
+      <c r="AB12" t="str">
+        <v/>
       </c>
       <c r="AC12" t="str">
         <v>Cirrhosis</v>
@@ -2637,6 +3957,54 @@
       <c r="F13" t="str">
         <v/>
       </c>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <v/>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <v/>
+      </c>
+      <c r="Q13" t="str">
+        <v/>
+      </c>
+      <c r="R13" t="str">
+        <v/>
+      </c>
+      <c r="S13" t="str">
+        <v/>
+      </c>
+      <c r="T13" t="str">
+        <v/>
+      </c>
+      <c r="U13" t="str">
+        <v/>
+      </c>
+      <c r="V13" t="str">
+        <v/>
+      </c>
       <c r="W13" t="str">
         <v>T3</v>
       </c>
@@ -2648,6 +4016,12 @@
       </c>
       <c r="Z13" t="str">
         <v>24.2</v>
+      </c>
+      <c r="AA13" t="str">
+        <v/>
+      </c>
+      <c r="AB13" t="str">
+        <v/>
       </c>
       <c r="AC13" t="str">
         <v>NephroticSyndrome</v>
@@ -2672,6 +4046,54 @@
       <c r="F14" t="str">
         <v/>
       </c>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <v/>
+      </c>
+      <c r="P14" t="str">
+        <v/>
+      </c>
+      <c r="Q14" t="str">
+        <v/>
+      </c>
+      <c r="R14" t="str">
+        <v/>
+      </c>
+      <c r="S14" t="str">
+        <v/>
+      </c>
+      <c r="T14" t="str">
+        <v/>
+      </c>
+      <c r="U14" t="str">
+        <v/>
+      </c>
+      <c r="V14" t="str">
+        <v/>
+      </c>
       <c r="W14" t="str">
         <v>FREET4</v>
       </c>
@@ -2683,6 +4105,12 @@
       </c>
       <c r="Z14" t="str">
         <v>237</v>
+      </c>
+      <c r="AA14" t="str">
+        <v/>
+      </c>
+      <c r="AB14" t="str">
+        <v/>
       </c>
       <c r="AC14" t="str">
         <v>AdvancedRenalFailure</v>
@@ -2695,10 +4123,64 @@
       <c r="B15" t="str">
         <v>60</v>
       </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v/>
+      </c>
       <c r="E15" t="str">
         <v/>
       </c>
       <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <v/>
+      </c>
+      <c r="O15" t="str">
+        <v/>
+      </c>
+      <c r="P15" t="str">
+        <v/>
+      </c>
+      <c r="Q15" t="str">
+        <v/>
+      </c>
+      <c r="R15" t="str">
+        <v/>
+      </c>
+      <c r="S15" t="str">
+        <v/>
+      </c>
+      <c r="T15" t="str">
+        <v/>
+      </c>
+      <c r="U15" t="str">
+        <v/>
+      </c>
+      <c r="V15" t="str">
         <v/>
       </c>
       <c r="W15" t="str">
@@ -2707,15 +4189,87 @@
       <c r="X15" t="str">
         <v>12.2</v>
       </c>
+      <c r="Y15" t="str">
+        <v/>
+      </c>
+      <c r="Z15" t="str">
+        <v/>
+      </c>
+      <c r="AA15" t="str">
+        <v/>
+      </c>
+      <c r="AB15" t="str">
+        <v/>
+      </c>
       <c r="AC15" t="str">
         <v>ResetOsmostat</v>
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="str">
+        <v/>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v/>
+      </c>
       <c r="E16" t="str">
         <v/>
       </c>
       <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16" t="str">
+        <v/>
+      </c>
+      <c r="O16" t="str">
+        <v/>
+      </c>
+      <c r="P16" t="str">
+        <v/>
+      </c>
+      <c r="Q16" t="str">
+        <v/>
+      </c>
+      <c r="R16" t="str">
+        <v/>
+      </c>
+      <c r="S16" t="str">
+        <v/>
+      </c>
+      <c r="T16" t="str">
+        <v/>
+      </c>
+      <c r="U16" t="str">
+        <v/>
+      </c>
+      <c r="V16" t="str">
         <v/>
       </c>
       <c r="W16" t="str">
@@ -2724,15 +4278,87 @@
       <c r="X16" t="str">
         <v>35</v>
       </c>
+      <c r="Y16" t="str">
+        <v/>
+      </c>
+      <c r="Z16" t="str">
+        <v/>
+      </c>
+      <c r="AA16" t="str">
+        <v/>
+      </c>
+      <c r="AB16" t="str">
+        <v/>
+      </c>
       <c r="AC16" t="str">
         <v>PrimaryPolydipsia</v>
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="str">
+        <v/>
+      </c>
+      <c r="B17" t="str">
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v/>
+      </c>
       <c r="E17" t="str">
         <v/>
       </c>
       <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <v/>
+      </c>
+      <c r="L17" t="str">
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17" t="str">
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <v/>
+      </c>
+      <c r="Q17" t="str">
+        <v/>
+      </c>
+      <c r="R17" t="str">
+        <v/>
+      </c>
+      <c r="S17" t="str">
+        <v/>
+      </c>
+      <c r="T17" t="str">
+        <v/>
+      </c>
+      <c r="U17" t="str">
+        <v/>
+      </c>
+      <c r="V17" t="str">
         <v/>
       </c>
       <c r="W17" t="str">
@@ -2741,15 +4367,87 @@
       <c r="X17" t="str">
         <v>30</v>
       </c>
+      <c r="Y17" t="str">
+        <v/>
+      </c>
+      <c r="Z17" t="str">
+        <v/>
+      </c>
+      <c r="AA17" t="str">
+        <v/>
+      </c>
+      <c r="AB17" t="str">
+        <v/>
+      </c>
       <c r="AC17" t="str">
         <v/>
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="str">
+        <v/>
+      </c>
+      <c r="B18" t="str">
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <v/>
+      </c>
       <c r="E18" t="str">
         <v/>
       </c>
       <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <v/>
+      </c>
+      <c r="L18" t="str">
+        <v/>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <v/>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
+      <c r="Q18" t="str">
+        <v/>
+      </c>
+      <c r="R18" t="str">
+        <v/>
+      </c>
+      <c r="S18" t="str">
+        <v/>
+      </c>
+      <c r="T18" t="str">
+        <v/>
+      </c>
+      <c r="U18" t="str">
+        <v/>
+      </c>
+      <c r="V18" t="str">
         <v/>
       </c>
       <c r="W18" t="str">
@@ -2758,15 +4456,105 @@
       <c r="X18" t="str">
         <v>3.6</v>
       </c>
+      <c r="Y18" t="str">
+        <v/>
+      </c>
+      <c r="Z18" t="str">
+        <v/>
+      </c>
+      <c r="AA18" t="str">
+        <v/>
+      </c>
+      <c r="AB18" t="str">
+        <v/>
+      </c>
       <c r="AC18" t="str">
         <v/>
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="str">
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
       <c r="E19" t="str">
         <v/>
       </c>
       <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <v/>
+      </c>
+      <c r="J19" t="str">
+        <v/>
+      </c>
+      <c r="K19" t="str">
+        <v/>
+      </c>
+      <c r="L19" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <v/>
+      </c>
+      <c r="Q19" t="str">
+        <v/>
+      </c>
+      <c r="R19" t="str">
+        <v/>
+      </c>
+      <c r="S19" t="str">
+        <v/>
+      </c>
+      <c r="T19" t="str">
+        <v/>
+      </c>
+      <c r="U19" t="str">
+        <v/>
+      </c>
+      <c r="V19" t="str">
+        <v/>
+      </c>
+      <c r="W19" t="str">
+        <v/>
+      </c>
+      <c r="X19" t="str">
+        <v/>
+      </c>
+      <c r="Y19" t="str">
+        <v/>
+      </c>
+      <c r="Z19" t="str">
+        <v/>
+      </c>
+      <c r="AA19" t="str">
+        <v/>
+      </c>
+      <c r="AB19" t="str">
         <v/>
       </c>
       <c r="AC19" t="str">
@@ -2774,10 +4562,88 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="str">
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <v/>
+      </c>
+      <c r="C20" t="str">
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
       <c r="E20" t="str">
         <v/>
       </c>
       <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <v/>
+      </c>
+      <c r="I20" t="str">
+        <v/>
+      </c>
+      <c r="J20" t="str">
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <v/>
+      </c>
+      <c r="L20" t="str">
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <v/>
+      </c>
+      <c r="N20" t="str">
+        <v/>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <v/>
+      </c>
+      <c r="Q20" t="str">
+        <v/>
+      </c>
+      <c r="R20" t="str">
+        <v/>
+      </c>
+      <c r="S20" t="str">
+        <v/>
+      </c>
+      <c r="T20" t="str">
+        <v/>
+      </c>
+      <c r="U20" t="str">
+        <v/>
+      </c>
+      <c r="V20" t="str">
+        <v/>
+      </c>
+      <c r="W20" t="str">
+        <v/>
+      </c>
+      <c r="X20" t="str">
+        <v/>
+      </c>
+      <c r="Y20" t="str">
+        <v/>
+      </c>
+      <c r="Z20" t="str">
+        <v/>
+      </c>
+      <c r="AA20" t="str">
+        <v/>
+      </c>
+      <c r="AB20" t="str">
         <v/>
       </c>
       <c r="AC20" t="str">

</xml_diff>